<commit_message>
Add more UserService and API
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Item #</t>
   </si>
@@ -84,13 +84,16 @@
   </si>
   <si>
     <t>Actual</t>
+  </si>
+  <si>
+    <t>In-progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +105,13 @@
       <b/>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -198,6 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +492,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,10 +575,12 @@
       <c r="D4" s="2">
         <v>43700</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2">
+        <v>43699</v>
+      </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
+      <c r="G4" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add API for book lending
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Item #</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>In-progress</t>
+  </si>
+  <si>
+    <t>Unit test</t>
   </si>
 </sst>
 </file>
@@ -202,13 +205,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,14 +510,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -579,7 +582,7 @@
         <v>43699</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -607,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2">
         <v>43717</v>
@@ -617,16 +620,14 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>43724</v>
@@ -642,13 +643,17 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43731</v>
+      </c>
+      <c r="D8" s="2">
+        <v>43735</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
@@ -657,10 +662,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -672,10 +677,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -687,16 +692,31 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
APIs to add Slug to books Angular to get book-detail by slug
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Item #</t>
   </si>
@@ -86,17 +86,17 @@
     <t>Actual</t>
   </si>
   <si>
-    <t>In-progress</t>
-  </si>
-  <si>
     <t>Unit test</t>
+  </si>
+  <si>
+    <t>Add more client pages to use APIs (Add new User/Book)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,14 +108,6 @@
       <b/>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -212,7 +204,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,7 +484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -605,9 +596,11 @@
       <c r="E5" s="2">
         <v>43705</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="9" t="s">
-        <v>20</v>
+      <c r="F5" s="2">
+        <v>43720</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -615,7 +608,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
         <v>43717</v>
@@ -625,7 +618,9 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -647,11 +642,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
         <v>43731</v>
@@ -667,13 +660,17 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43738</v>
+      </c>
+      <c r="D9" s="2">
+        <v>43742</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
@@ -682,13 +679,17 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43745</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43749</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
@@ -697,13 +698,17 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43752</v>
+      </c>
+      <c r="D11" s="2">
+        <v>43756</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
@@ -712,16 +717,35 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43759</v>
+      </c>
+      <c r="D12" s="2">
+        <v>43763</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add unit test for BooksApiController
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Item #</t>
   </si>
@@ -90,13 +90,16 @@
   </si>
   <si>
     <t>Add more client pages to use APIs (Add new User/Book)</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +111,13 @@
       <b/>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -204,6 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +627,12 @@
       <c r="D6" s="2">
         <v>43721</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2">
+        <v>43724</v>
+      </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
+      <c r="G6" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Complete Unit Test for BookLendingApiController
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Item #</t>
   </si>
@@ -90,16 +90,13 @@
   </si>
   <si>
     <t>Add more client pages to use APIs (Add new User/Book)</t>
-  </si>
-  <si>
-    <t>In-Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,13 +108,6 @@
       <b/>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -214,7 +204,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +487,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,9 +619,11 @@
       <c r="E6" s="2">
         <v>43724</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="9" t="s">
-        <v>22</v>
+      <c r="F6" s="2">
+        <v>43727</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add docker file and docker compose
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Item #</t>
   </si>
@@ -90,13 +90,16 @@
   </si>
   <si>
     <t>Add more client pages to use APIs (Add new User/Book)</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +111,13 @@
       <b/>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -204,6 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,7 +498,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,10 +650,12 @@
       <c r="D7" s="2">
         <v>43728</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="2">
+        <v>43731</v>
+      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
+      <c r="G7" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add docker, docker-compose local
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -208,13 +208,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,14 +513,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -653,9 +653,11 @@
       <c r="E7" s="2">
         <v>43731</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="9" t="s">
-        <v>22</v>
+      <c r="F7" s="2">
+        <v>43740</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -669,10 +671,12 @@
       <c r="D8" s="2">
         <v>43735</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="2">
+        <v>43741</v>
+      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
+      <c r="G8" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Testing build with triggering from Github
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\KPIs\2019\anhnguyen-kpi-2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\KPIs\2019\GitHub_Repo\anhnguyen-kpi-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,8 +675,8 @@
         <v>43741</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="7" t="s">
-        <v>22</v>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -694,8 +694,8 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
+      <c r="G9" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -713,8 +713,8 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
+      <c r="G10" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -732,8 +732,8 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
+      <c r="G11" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>